<commit_message>
Made the numbers integers.
</commit_message>
<xml_diff>
--- a/data/workbook1.xlsx
+++ b/data/workbook1.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="279" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="237">
   <si>
     <t>Region sends troops to rescue Central African regime</t>
   </si>
@@ -724,6 +724,15 @@
   </si>
   <si>
     <t>Number of People Affected, Areas Affected, Number of People Killed</t>
+  </si>
+  <si>
+    <t>People Affected, People Killed, Houses Affected</t>
+  </si>
+  <si>
+    <t>Government of Bolivia (Ministerio de Defensa)</t>
+  </si>
+  <si>
+    <t>Bolivia</t>
   </si>
 </sst>
 </file>
@@ -1134,8 +1143,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C38" workbookViewId="0">
-      <selection activeCell="H48" sqref="H48"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -2391,6 +2400,18 @@
       <c r="E50" s="3" t="s">
         <v>97</v>
       </c>
+      <c r="F50" t="s">
+        <v>158</v>
+      </c>
+      <c r="G50" t="s">
+        <v>229</v>
+      </c>
+      <c r="I50" t="s">
+        <v>195</v>
+      </c>
+      <c r="J50" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="51" spans="1:10" ht="16">
       <c r="A51" s="1">
@@ -2441,6 +2462,21 @@
       </c>
       <c r="E53" s="3" t="s">
         <v>103</v>
+      </c>
+      <c r="F53" t="s">
+        <v>234</v>
+      </c>
+      <c r="G53" t="s">
+        <v>229</v>
+      </c>
+      <c r="H53" t="s">
+        <v>235</v>
+      </c>
+      <c r="I53" t="s">
+        <v>236</v>
+      </c>
+      <c r="J53" t="s">
+        <v>189</v>
       </c>
     </row>
     <row r="54" spans="1:10" ht="16">

</xml_diff>